<commit_message>
update submap to upel
</commit_message>
<xml_diff>
--- a/gee/stat.xlsx
+++ b/gee/stat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au686295\Documents\GitHub\PhD\orbit-drift-MODIS-ice-albedo\gee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187342BF-5575-4F81-91B0-E6BB89F2390B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7A400C-04A4-4767-94E8-0A781E21FBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{49D7E878-2DD4-473C-8D14-502A01B15A7E}"/>
   </bookViews>
@@ -3511,10 +3511,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62101249-8DDD-44BD-9CE3-E155592038DC}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3522,7 +3522,7 @@
     <col min="1" max="1" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13">
         <v>2000</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>7.5499999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13">
         <v>2001</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>0.1086</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>2002</v>
       </c>
@@ -3592,8 +3592,12 @@
         <f>MEDIAN(B4:B20)</f>
         <v>3.9199999999999999E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <f>_xlfn.STDEV.P(B4:B20)</f>
+        <v>2.6288224105929986E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>2003</v>
       </c>
@@ -3602,7 +3606,7 @@
       </c>
       <c r="C5" s="18"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>2004</v>
       </c>
@@ -3611,7 +3615,7 @@
       </c>
       <c r="C6" s="18"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>2005</v>
       </c>
@@ -3620,7 +3624,7 @@
       </c>
       <c r="C7" s="18"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>2006</v>
       </c>
@@ -3629,7 +3633,7 @@
       </c>
       <c r="C8" s="18"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>2007</v>
       </c>
@@ -3638,7 +3642,7 @@
       </c>
       <c r="C9" s="18"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>2008</v>
       </c>
@@ -3647,7 +3651,7 @@
       </c>
       <c r="C10" s="9"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>2009</v>
       </c>
@@ -3656,7 +3660,7 @@
       </c>
       <c r="C11" s="9"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>2010</v>
       </c>
@@ -3665,7 +3669,7 @@
       </c>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>2011</v>
       </c>
@@ -3674,7 +3678,7 @@
       </c>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>2012</v>
       </c>
@@ -3683,7 +3687,7 @@
       </c>
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>2013</v>
       </c>
@@ -3693,7 +3697,7 @@
       <c r="C15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>2014</v>
       </c>

</xml_diff>